<commit_message>
Add system diagram to requirements analysis.
</commit_message>
<xml_diff>
--- a/01-requirements/Requirements Analysis.xlsx
+++ b/01-requirements/Requirements Analysis.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korwinula\Dropbox\electronics\complete\MIDI Router MCU\01 - Define\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/korwinan/sandbox/MIDI-Router/01-requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3FE756BB-6256-48E2-A801-A29DB0F4F94A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{DCE50D8A-037B-7240-BEB8-F97F54B9E1D0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9050" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30120" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Fabric Utilization" sheetId="1" r:id="rId1"/>
-    <sheet name="FPGA Pin Use" sheetId="5" r:id="rId2"/>
-    <sheet name="PIC24" sheetId="4" r:id="rId3"/>
-    <sheet name="Requirements-QFD1" sheetId="3" r:id="rId4"/>
+    <sheet name="System Diagram" sheetId="6" r:id="rId1"/>
+    <sheet name="Fabric Utilization" sheetId="1" r:id="rId2"/>
+    <sheet name="FPGA Pin Use" sheetId="5" r:id="rId3"/>
+    <sheet name="PIC24" sheetId="4" r:id="rId4"/>
+    <sheet name="Requirements-QFD1" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'FPGA Pin Use'!$A$4:$H$155</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'FPGA Pin Use'!$A$4:$H$155</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="427">
   <si>
     <t>Pin Count</t>
   </si>
@@ -1265,6 +1266,99 @@
   </si>
   <si>
     <t>FBIN0</t>
+  </si>
+  <si>
+    <t>UART data</t>
+  </si>
+  <si>
+    <t>UART interrupt</t>
+  </si>
+  <si>
+    <t>mute outputs</t>
+  </si>
+  <si>
+    <t>switch matrix</t>
+  </si>
+  <si>
+    <t>MCU</t>
+  </si>
+  <si>
+    <t>FPGA</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Functional I/O</t>
+  </si>
+  <si>
+    <t>Clock</t>
+  </si>
+  <si>
+    <t>spare</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>CDC class</t>
+  </si>
+  <si>
+    <t>MIDI input</t>
+  </si>
+  <si>
+    <t>Ch A</t>
+  </si>
+  <si>
+    <t>Ch B</t>
+  </si>
+  <si>
+    <t>Ch C</t>
+  </si>
+  <si>
+    <t>Ch D</t>
+  </si>
+  <si>
+    <t>MIDI Output</t>
+  </si>
+  <si>
+    <t>I2C</t>
+  </si>
+  <si>
+    <t>NV memory</t>
+  </si>
+  <si>
+    <t>LED's 1-8</t>
+  </si>
+  <si>
+    <t>LED's 9-16</t>
+  </si>
+  <si>
+    <t>PB's 1-8</t>
+  </si>
+  <si>
+    <t>PB's 9-16</t>
+  </si>
+  <si>
+    <t>MIDI Input</t>
+  </si>
+  <si>
+    <t>MIDI Thru</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>1.2V</t>
+  </si>
+  <si>
+    <t>120 VAC</t>
   </si>
 </sst>
 </file>
@@ -1384,7 +1478,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1460,11 +1554,171 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1520,9 +1774,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1531,6 +1782,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1549,6 +1848,629 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF6C339B-A922-7F46-9DC9-0C540515067F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10833100" y="1257300"/>
+          <a:ext cx="3327400" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20112C18-6E83-9A43-9F88-A1F8C5E7A193}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10883900" y="2222500"/>
+          <a:ext cx="3238500" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8943B18-423E-164D-A673-58324D2EE42B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10858500" y="3530600"/>
+          <a:ext cx="3276600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8B407D6-1234-5045-B51F-0DEB06533D46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10896600" y="4953000"/>
+          <a:ext cx="3276600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADE7303F-AE6E-7745-9054-50F21D7EBEF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10464800" y="2679700"/>
+          <a:ext cx="0" cy="177800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12826</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>12575</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>126</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3605B3DB-6C10-DD44-9561-6D4E5D10A780}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4162331" y="2464554"/>
+          <a:ext cx="2690640" cy="126"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>817327</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1760</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BBE8849-E4E1-8B42-A9D3-9B55DE2F7CEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4174905" y="3407624"/>
+          <a:ext cx="2652917" cy="1760"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12575</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>176040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>804753</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA821340-4A36-CE48-8CE4-50E20931DFF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4162080" y="4526733"/>
+          <a:ext cx="2653168" cy="12575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>817327</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80BD2B2B-8F71-DA41-9E66-048597460F6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4149505" y="4916535"/>
+          <a:ext cx="2678317" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>817328</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>12574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>12576</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Straight Arrow Connector 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFE29BCE-D414-FF46-8978-E76C837511BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7657724" y="1911287"/>
+          <a:ext cx="2502276" cy="2"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>12574</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>817327</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71444A66-DFD0-7E40-BE62-B7FF8D5CDCF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7682871" y="4539307"/>
+          <a:ext cx="2464555" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2632,6 +3554,600 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8268F9F-964F-594F-B2B4-2D91C8B5EC04}">
+  <dimension ref="C4:R36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C4" s="29"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="31"/>
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C5" s="24"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="33" t="s">
+        <v>423</v>
+      </c>
+      <c r="M5" s="32"/>
+    </row>
+    <row r="6" spans="3:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="24"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="33" t="s">
+        <v>424</v>
+      </c>
+      <c r="M6" s="32"/>
+      <c r="R6" s="40" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="7" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C7" s="24"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="33" t="s">
+        <v>425</v>
+      </c>
+      <c r="M7" s="43" t="s">
+        <v>423</v>
+      </c>
+      <c r="R7" s="49" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="8" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C8" s="24"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="33"/>
+      <c r="M8" s="44"/>
+    </row>
+    <row r="9" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C9" s="24"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="33" t="s">
+        <v>423</v>
+      </c>
+      <c r="M9" s="45" t="s">
+        <v>423</v>
+      </c>
+      <c r="R9" s="40" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="10" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C10" s="24"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="J10" s="32"/>
+      <c r="K10" s="33" t="s">
+        <v>409</v>
+      </c>
+      <c r="M10" s="44" t="s">
+        <v>421</v>
+      </c>
+      <c r="R10" s="42" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="11" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C11" s="24"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32" t="s">
+        <v>403</v>
+      </c>
+      <c r="H11" s="32"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="34" t="s">
+        <v>410</v>
+      </c>
+      <c r="M11" s="47" t="s">
+        <v>410</v>
+      </c>
+      <c r="R11" s="50" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="12" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C12" s="24"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="35" t="s">
+        <v>368</v>
+      </c>
+      <c r="H12" s="32"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="34" t="s">
+        <v>411</v>
+      </c>
+      <c r="M12" s="47" t="s">
+        <v>411</v>
+      </c>
+      <c r="R12" s="50" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="13" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C13" s="24"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="32"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="34" t="s">
+        <v>412</v>
+      </c>
+      <c r="M13" s="47" t="s">
+        <v>412</v>
+      </c>
+      <c r="R13" s="50" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="14" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C14" s="24"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="34" t="s">
+        <v>413</v>
+      </c>
+      <c r="M14" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="R14" s="49" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="15" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C15" s="24"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="32"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="33"/>
+      <c r="M15" s="44"/>
+      <c r="R15" s="41"/>
+    </row>
+    <row r="16" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C16" s="24"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="35" t="s">
+        <v>396</v>
+      </c>
+      <c r="H16" s="32"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="33"/>
+      <c r="M16" s="45" t="s">
+        <v>423</v>
+      </c>
+      <c r="R16" s="40" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C17" s="24" t="s">
+        <v>402</v>
+      </c>
+      <c r="D17" s="32"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="35" t="s">
+        <v>399</v>
+      </c>
+      <c r="H17" s="32"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="34"/>
+      <c r="M17" s="44" t="s">
+        <v>422</v>
+      </c>
+      <c r="R17" s="42" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C18" s="24"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="35" t="s">
+        <v>398</v>
+      </c>
+      <c r="H18" s="32"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="34"/>
+      <c r="M18" s="47" t="s">
+        <v>410</v>
+      </c>
+      <c r="R18" s="50" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C19" s="24" t="s">
+        <v>407</v>
+      </c>
+      <c r="D19" s="32"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="34"/>
+      <c r="M19" s="47" t="s">
+        <v>411</v>
+      </c>
+      <c r="R19" s="50" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C20" s="36" t="s">
+        <v>408</v>
+      </c>
+      <c r="D20" s="32"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32" t="s">
+        <v>404</v>
+      </c>
+      <c r="H20" s="32"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="34"/>
+      <c r="M20" s="47" t="s">
+        <v>412</v>
+      </c>
+      <c r="R20" s="50" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="21" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C21" s="24"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="H21" s="32"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="33"/>
+      <c r="M21" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="R21" s="49" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="22" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C22" s="24"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="35" t="s">
+        <v>406</v>
+      </c>
+      <c r="H22" s="32"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="33"/>
+      <c r="M22" s="44"/>
+      <c r="R22" s="41"/>
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C23" s="24"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="35" t="s">
+        <v>406</v>
+      </c>
+      <c r="H23" s="32"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="33" t="s">
+        <v>423</v>
+      </c>
+      <c r="M23" s="45" t="s">
+        <v>423</v>
+      </c>
+      <c r="R23" s="40" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C24" s="24"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="35" t="s">
+        <v>406</v>
+      </c>
+      <c r="H24" s="32"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="33" t="s">
+        <v>414</v>
+      </c>
+      <c r="M24" s="44" t="s">
+        <v>414</v>
+      </c>
+      <c r="R24" s="42" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C25" s="24"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="34" t="s">
+        <v>410</v>
+      </c>
+      <c r="M25" s="47" t="s">
+        <v>410</v>
+      </c>
+      <c r="R25" s="50" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C26" s="24"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32" t="s">
+        <v>405</v>
+      </c>
+      <c r="H26" s="32"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="34" t="s">
+        <v>411</v>
+      </c>
+      <c r="M26" s="47" t="s">
+        <v>411</v>
+      </c>
+      <c r="R26" s="50" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C27" s="24"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="34" t="s">
+        <v>412</v>
+      </c>
+      <c r="M27" s="47" t="s">
+        <v>412</v>
+      </c>
+      <c r="R27" s="50" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C28" s="24"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="34" t="s">
+        <v>413</v>
+      </c>
+      <c r="M28" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="R28" s="49" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="29" spans="3:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="24"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="33"/>
+      <c r="M29" s="46"/>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C30" s="24"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="33" t="s">
+        <v>415</v>
+      </c>
+      <c r="R30" s="41"/>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C31" s="24"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="34" t="s">
+        <v>416</v>
+      </c>
+      <c r="R31" s="41"/>
+    </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C32" s="24"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="34" t="s">
+        <v>417</v>
+      </c>
+      <c r="R32" s="41"/>
+    </row>
+    <row r="33" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C33" s="24"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="34" t="s">
+        <v>418</v>
+      </c>
+      <c r="R33" s="41"/>
+    </row>
+    <row r="34" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C34" s="24"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="34" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="35" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C35" s="24"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="34" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="36" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C36" s="37"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I10:I33"/>
+    <mergeCell ref="E11:E27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -2639,12 +4155,12 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2658,7 +4174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2674,7 +4190,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>153</v>
       </c>
@@ -2689,7 +4205,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>154</v>
       </c>
@@ -2704,7 +4220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -2719,7 +4235,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>156</v>
       </c>
@@ -2734,7 +4250,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -2749,7 +4265,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>158</v>
       </c>
@@ -2764,7 +4280,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>152</v>
       </c>
@@ -2779,7 +4295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -2794,7 +4310,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2810,7 +4326,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>0</v>
       </c>
@@ -2822,7 +4338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2837,7 +4353,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -2846,7 +4362,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -2854,7 +4370,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -2870,36 +4386,36 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63F63D7-D9E5-44DC-B22E-D22BA96211A0}">
   <sheetPr filterMode="1"/>
   <dimension ref="A3:H155"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="G4" sqref="G4"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" ht="58.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="21" t="s">
+    <row r="3" spans="1:8" ht="58.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+    </row>
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>391</v>
       </c>
@@ -2925,7 +4441,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -2948,7 +4464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -2971,7 +4487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -2994,7 +4510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -3017,7 +4533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>106</v>
       </c>
@@ -3040,7 +4556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>130</v>
       </c>
@@ -3063,7 +4579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>5</v>
       </c>
@@ -3086,7 +4602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>6</v>
       </c>
@@ -3109,7 +4625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>9</v>
       </c>
@@ -3132,7 +4648,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -3155,7 +4671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>119</v>
       </c>
@@ -3178,7 +4694,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>11</v>
       </c>
@@ -3201,7 +4717,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>12</v>
       </c>
@@ -3227,7 +4743,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>131</v>
       </c>
@@ -3250,7 +4766,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>13</v>
       </c>
@@ -3276,7 +4792,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>14</v>
       </c>
@@ -3302,7 +4818,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>113</v>
       </c>
@@ -3325,7 +4841,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>15</v>
       </c>
@@ -3351,7 +4867,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>16</v>
       </c>
@@ -3377,7 +4893,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>19</v>
       </c>
@@ -3403,7 +4919,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>20</v>
       </c>
@@ -3429,7 +4945,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>132</v>
       </c>
@@ -3452,7 +4968,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>114</v>
       </c>
@@ -3475,7 +4991,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>23</v>
       </c>
@@ -3501,7 +5017,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>24</v>
       </c>
@@ -3527,7 +5043,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -3553,7 +5069,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -3579,7 +5095,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -3605,7 +5121,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -3631,7 +5147,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -3657,7 +5173,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>128</v>
       </c>
@@ -3680,7 +5196,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>107</v>
       </c>
@@ -3703,7 +5219,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>37</v>
       </c>
@@ -3729,7 +5245,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>38</v>
       </c>
@@ -3755,7 +5271,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>120</v>
       </c>
@@ -3778,7 +5294,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -3804,7 +5320,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -3830,7 +5346,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>129</v>
       </c>
@@ -3853,7 +5369,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>108</v>
       </c>
@@ -3876,7 +5392,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44</v>
       </c>
@@ -3902,7 +5418,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>45</v>
       </c>
@@ -3928,7 +5444,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>46</v>
       </c>
@@ -3954,7 +5470,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>47</v>
       </c>
@@ -3980,7 +5496,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>48</v>
       </c>
@@ -4006,7 +5522,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>49</v>
       </c>
@@ -4028,11 +5544,11 @@
       <c r="G49" s="2">
         <v>67</v>
       </c>
-      <c r="H49" s="23" t="s">
+      <c r="H49" s="22" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>50</v>
       </c>
@@ -4054,11 +5570,11 @@
       <c r="G50" s="2">
         <v>68</v>
       </c>
-      <c r="H50" s="23" t="s">
+      <c r="H50" s="22" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>109</v>
       </c>
@@ -4081,7 +5597,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -4103,11 +5619,11 @@
       <c r="G52" s="2">
         <v>70</v>
       </c>
-      <c r="H52" s="23" t="s">
+      <c r="H52" s="22" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -4133,7 +5649,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -4155,9 +5671,9 @@
       <c r="G54" s="2">
         <v>72</v>
       </c>
-      <c r="H54" s="24"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H54" s="23"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>59</v>
       </c>
@@ -4179,9 +5695,9 @@
       <c r="G55" s="2">
         <v>78</v>
       </c>
-      <c r="H55" s="24"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H55" s="23"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>60</v>
       </c>
@@ -4203,9 +5719,9 @@
       <c r="G56" s="2">
         <v>79</v>
       </c>
-      <c r="H56" s="25"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H56" s="24"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>61</v>
       </c>
@@ -4228,7 +5744,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>62</v>
       </c>
@@ -4251,7 +5767,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>110</v>
       </c>
@@ -4274,7 +5790,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>63</v>
       </c>
@@ -4297,7 +5813,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>64</v>
       </c>
@@ -4320,7 +5836,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>126</v>
       </c>
@@ -4343,7 +5859,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>65</v>
       </c>
@@ -4366,7 +5882,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>66</v>
       </c>
@@ -4389,7 +5905,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>121</v>
       </c>
@@ -4412,7 +5928,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>67</v>
       </c>
@@ -4435,7 +5951,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>68</v>
       </c>
@@ -4458,7 +5974,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>70</v>
       </c>
@@ -4481,7 +5997,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>71</v>
       </c>
@@ -4504,7 +6020,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>72</v>
       </c>
@@ -4527,7 +6043,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>127</v>
       </c>
@@ -4550,7 +6066,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>74</v>
       </c>
@@ -4573,7 +6089,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>75</v>
       </c>
@@ -4596,7 +6112,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>111</v>
       </c>
@@ -4619,7 +6135,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>76</v>
       </c>
@@ -4642,7 +6158,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>77</v>
       </c>
@@ -4665,7 +6181,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>78</v>
       </c>
@@ -4688,7 +6204,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>79</v>
       </c>
@@ -4711,7 +6227,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>80</v>
       </c>
@@ -4734,7 +6250,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>81</v>
       </c>
@@ -4757,7 +6273,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>122</v>
       </c>
@@ -4780,7 +6296,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>82</v>
       </c>
@@ -4803,7 +6319,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>83</v>
       </c>
@@ -4826,7 +6342,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>84</v>
       </c>
@@ -4849,7 +6365,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>86</v>
       </c>
@@ -4872,7 +6388,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>87</v>
       </c>
@@ -4895,7 +6411,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>88</v>
       </c>
@@ -4918,7 +6434,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>115</v>
       </c>
@@ -4941,7 +6457,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>89</v>
       </c>
@@ -4964,7 +6480,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>90</v>
       </c>
@@ -4987,7 +6503,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>91</v>
       </c>
@@ -5010,7 +6526,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>125</v>
       </c>
@@ -5033,7 +6549,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>93</v>
       </c>
@@ -5056,7 +6572,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>94</v>
       </c>
@@ -5079,7 +6595,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>95</v>
       </c>
@@ -5102,7 +6618,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>124</v>
       </c>
@@ -5125,7 +6641,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -5148,7 +6664,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -5171,7 +6687,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -5194,7 +6710,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -5217,7 +6733,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -5240,7 +6756,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>112</v>
       </c>
@@ -5263,7 +6779,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -5286,7 +6802,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>104</v>
       </c>
@@ -5309,7 +6825,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>7</v>
       </c>
@@ -5332,7 +6848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>8</v>
       </c>
@@ -5355,7 +6871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>17</v>
       </c>
@@ -5378,7 +6894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>18</v>
       </c>
@@ -5401,7 +6917,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>21</v>
       </c>
@@ -5424,7 +6940,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>22</v>
       </c>
@@ -5447,11 +6963,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>25</v>
       </c>
-      <c r="B111" s="22" t="s">
+      <c r="B111" s="21" t="s">
         <v>186</v>
       </c>
       <c r="C111" s="2" t="s">
@@ -5470,11 +6986,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>26</v>
       </c>
-      <c r="B112" s="22" t="s">
+      <c r="B112" s="21" t="s">
         <v>188</v>
       </c>
       <c r="C112" s="2" t="s">
@@ -5493,7 +7009,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>27</v>
       </c>
@@ -5516,7 +7032,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>28</v>
       </c>
@@ -5539,7 +7055,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>34</v>
       </c>
@@ -5562,7 +7078,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>35</v>
       </c>
@@ -5585,7 +7101,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>36</v>
       </c>
@@ -5608,7 +7124,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>41</v>
       </c>
@@ -5631,7 +7147,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>42</v>
       </c>
@@ -5654,7 +7170,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>43</v>
       </c>
@@ -5677,7 +7193,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>54</v>
       </c>
@@ -5700,7 +7216,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>55</v>
       </c>
@@ -5723,7 +7239,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>56</v>
       </c>
@@ -5746,7 +7262,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>57</v>
       </c>
@@ -5769,7 +7285,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>58</v>
       </c>
@@ -5792,7 +7308,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>69</v>
       </c>
@@ -5815,7 +7331,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>73</v>
       </c>
@@ -5838,7 +7354,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>85</v>
       </c>
@@ -5861,7 +7377,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>92</v>
       </c>
@@ -5884,7 +7400,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>101</v>
       </c>
@@ -5907,7 +7423,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>103</v>
       </c>
@@ -5930,7 +7446,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>105</v>
       </c>
@@ -5953,7 +7469,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>116</v>
       </c>
@@ -5976,7 +7492,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>117</v>
       </c>
@@ -5999,7 +7515,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>118</v>
       </c>
@@ -6022,7 +7538,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>123</v>
       </c>
@@ -6045,7 +7561,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>133</v>
       </c>
@@ -6068,7 +7584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>134</v>
       </c>
@@ -6091,7 +7607,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>135</v>
       </c>
@@ -6114,7 +7630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>136</v>
       </c>
@@ -6137,7 +7653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>137</v>
       </c>
@@ -6160,7 +7676,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>138</v>
       </c>
@@ -6183,7 +7699,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
         <v>139</v>
       </c>
@@ -6206,7 +7722,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>140</v>
       </c>
@@ -6229,7 +7745,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>141</v>
       </c>
@@ -6252,7 +7768,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>142</v>
       </c>
@@ -6275,7 +7791,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
         <v>143</v>
       </c>
@@ -6298,7 +7814,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>144</v>
       </c>
@@ -6321,7 +7837,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
         <v>145</v>
       </c>
@@ -6344,7 +7860,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>146</v>
       </c>
@@ -6367,7 +7883,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
         <v>147</v>
       </c>
@@ -6390,7 +7906,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>148</v>
       </c>
@@ -6413,7 +7929,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <v>149</v>
       </c>
@@ -6436,7 +7952,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>150</v>
       </c>
@@ -6459,7 +7975,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
         <v>151</v>
       </c>
@@ -6600,7 +8116,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
@@ -6608,16 +8124,16 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="15"/>
-    <col min="2" max="2" width="71.08984375" style="15" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.36328125" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.90625" style="15"/>
+    <col min="1" max="1" width="8.83203125" style="15"/>
+    <col min="2" max="2" width="71.1640625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>86</v>
       </c>
@@ -6631,7 +8147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -6642,7 +8158,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -6656,7 +8172,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -6670,7 +8186,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -6684,7 +8200,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -6696,7 +8212,7 @@
       </c>
       <c r="D6" s="16"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -6704,7 +8220,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -6712,7 +8228,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -6726,7 +8242,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -6740,7 +8256,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -6751,7 +8267,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -6762,7 +8278,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -6773,7 +8289,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -6784,7 +8300,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -6792,7 +8308,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="15">
         <v>15</v>
       </c>
@@ -6800,7 +8316,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -6811,7 +8327,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -6822,7 +8338,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -6833,7 +8349,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -6844,7 +8360,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -6855,7 +8371,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -6866,7 +8382,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -6877,7 +8393,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -6888,7 +8404,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -6899,7 +8415,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -6910,7 +8426,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -6921,7 +8437,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -6930,7 +8446,7 @@
       </c>
       <c r="D28" s="16"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -6941,7 +8457,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -6952,7 +8468,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -6960,7 +8476,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -6968,7 +8484,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -6979,7 +8495,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -6993,7 +8509,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -7007,7 +8523,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -7021,7 +8537,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -7035,7 +8551,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -7049,7 +8565,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -7063,7 +8579,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -7071,7 +8587,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -7079,7 +8595,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -7090,7 +8606,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -7104,7 +8620,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -7118,7 +8634,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -7129,12 +8645,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="D47" s="18" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D48" s="16"/>
     </row>
   </sheetData>
@@ -7142,38 +8658,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.08984375" style="13" customWidth="1"/>
-    <col min="2" max="3" width="8.90625" style="13"/>
-    <col min="4" max="4" width="10.453125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.6328125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="6.1796875" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.1796875" style="13" customWidth="1"/>
-    <col min="8" max="8" width="6.36328125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="6.1796875" style="13" customWidth="1"/>
-    <col min="10" max="11" width="8.90625" style="13"/>
-    <col min="12" max="13" width="6.1796875" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.90625" style="13"/>
+    <col min="1" max="1" width="27.1640625" style="13" customWidth="1"/>
+    <col min="2" max="3" width="8.83203125" style="13"/>
+    <col min="4" max="4" width="10.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.1640625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" style="13" customWidth="1"/>
+    <col min="9" max="9" width="6.1640625" style="13" customWidth="1"/>
+    <col min="10" max="11" width="8.83203125" style="13"/>
+    <col min="12" max="13" width="6.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E1" s="13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="119.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="119.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E2" s="17" t="s">
         <v>132</v>
       </c>
@@ -7202,7 +8718,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>80</v>
       </c>
@@ -7210,7 +8726,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>142</v>
       </c>
@@ -7233,7 +8749,7 @@
       <c r="L4" s="19"/>
       <c r="M4" s="19"/>
     </row>
-    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>83</v>
       </c>
@@ -7252,7 +8768,7 @@
       <c r="L5" s="19"/>
       <c r="M5" s="19"/>
     </row>
-    <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>84</v>
       </c>
@@ -7271,7 +8787,7 @@
       <c r="L6" s="19"/>
       <c r="M6" s="19"/>
     </row>
-    <row r="7" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>85</v>
       </c>
@@ -7290,7 +8806,7 @@
       <c r="L7" s="19"/>
       <c r="M7" s="19"/>
     </row>
-    <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>143</v>
       </c>
@@ -7309,7 +8825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>145</v>
       </c>
@@ -7328,7 +8844,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>146</v>
       </c>
@@ -7349,7 +8865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>147</v>
       </c>
@@ -7370,7 +8886,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>144</v>
       </c>
@@ -7391,7 +8907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>148</v>
       </c>
@@ -7410,7 +8926,7 @@
       </c>
       <c r="M13" s="19"/>
     </row>
-    <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>149</v>
       </c>
@@ -7429,7 +8945,7 @@
       </c>
       <c r="M14" s="19"/>
     </row>
-    <row r="15" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>139</v>
       </c>
@@ -7450,7 +8966,7 @@
       </c>
       <c r="M15" s="19"/>
     </row>
-    <row r="16" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>150</v>
       </c>
@@ -7467,7 +8983,7 @@
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
         <v>151</v>
       </c>
@@ -7484,7 +9000,7 @@
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E19" s="13">
         <f>SUMPRODUCT($D4:$D17, E4:E17)</f>
         <v>40</v>

</xml_diff>

<commit_message>
Update requirements analysis. Complete first pass at signal conditioner board. Add power analysis.
</commit_message>
<xml_diff>
--- a/01-requirements/Requirements Analysis.xlsx
+++ b/01-requirements/Requirements Analysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/korwinan/sandbox/MIDI-Router/01-requirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korwinula\Documents\MIDI-Router\01-requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{DCE50D8A-037B-7240-BEB8-F97F54B9E1D0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0BFE3CB5-DF6E-4CAE-8275-201822F71AEA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30120" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1782,18 +1782,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1829,6 +1817,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3557,585 +3557,585 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8268F9F-964F-594F-B2B4-2D91C8B5EC04}">
   <dimension ref="C4:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="101" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C4" s="29"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
-    </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="27"/>
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C5" s="24"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="33" t="s">
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="29" t="s">
         <v>423</v>
       </c>
-      <c r="M5" s="32"/>
-    </row>
-    <row r="6" spans="3:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="28"/>
+    </row>
+    <row r="6" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C6" s="24"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="33" t="s">
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="29" t="s">
         <v>424</v>
       </c>
-      <c r="M6" s="32"/>
-      <c r="R6" s="40" t="s">
+      <c r="M6" s="28"/>
+      <c r="R6" s="36" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C7" s="24"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="33" t="s">
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29" t="s">
         <v>425</v>
       </c>
-      <c r="M7" s="43" t="s">
+      <c r="M7" s="39" t="s">
         <v>423</v>
       </c>
-      <c r="R7" s="49" t="s">
+      <c r="R7" s="45" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C8" s="24"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="33"/>
-      <c r="M8" s="44"/>
-    </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
+      <c r="M8" s="40"/>
+    </row>
+    <row r="9" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C9" s="24"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="33" t="s">
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29" t="s">
         <v>423</v>
       </c>
-      <c r="M9" s="45" t="s">
+      <c r="M9" s="41" t="s">
         <v>423</v>
       </c>
-      <c r="R9" s="40" t="s">
+      <c r="R9" s="36" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C10" s="24"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="26" t="s">
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="47" t="s">
         <v>401</v>
       </c>
-      <c r="J10" s="32"/>
-      <c r="K10" s="33" t="s">
+      <c r="J10" s="28"/>
+      <c r="K10" s="29" t="s">
         <v>409</v>
       </c>
-      <c r="M10" s="44" t="s">
+      <c r="M10" s="40" t="s">
         <v>421</v>
       </c>
-      <c r="R10" s="42" t="s">
+      <c r="R10" s="38" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C11" s="24"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="26" t="s">
+      <c r="D11" s="28"/>
+      <c r="E11" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32" t="s">
+      <c r="F11" s="28"/>
+      <c r="G11" s="28" t="s">
         <v>403</v>
       </c>
-      <c r="H11" s="32"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="34" t="s">
+      <c r="H11" s="28"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="30" t="s">
         <v>410</v>
       </c>
-      <c r="M11" s="47" t="s">
+      <c r="M11" s="43" t="s">
         <v>410</v>
       </c>
-      <c r="R11" s="50" t="s">
+      <c r="R11" s="46" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C12" s="24"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="35" t="s">
+      <c r="D12" s="28"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="31" t="s">
         <v>368</v>
       </c>
-      <c r="H12" s="32"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="34" t="s">
+      <c r="H12" s="28"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="30" t="s">
         <v>411</v>
       </c>
-      <c r="M12" s="47" t="s">
+      <c r="M12" s="43" t="s">
         <v>411</v>
       </c>
-      <c r="R12" s="50" t="s">
+      <c r="R12" s="46" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C13" s="24"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="35" t="s">
+      <c r="D13" s="28"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="32"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="34" t="s">
+      <c r="H13" s="28"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="30" t="s">
         <v>412</v>
       </c>
-      <c r="M13" s="47" t="s">
+      <c r="M13" s="43" t="s">
         <v>412</v>
       </c>
-      <c r="R13" s="50" t="s">
+      <c r="R13" s="46" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C14" s="24"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="34" t="s">
+      <c r="D14" s="28"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="30" t="s">
         <v>413</v>
       </c>
-      <c r="M14" s="48" t="s">
+      <c r="M14" s="44" t="s">
         <v>413</v>
       </c>
-      <c r="R14" s="49" t="s">
+      <c r="R14" s="45" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C15" s="24"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32" t="s">
+      <c r="D15" s="28"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="32"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="33"/>
-      <c r="M15" s="44"/>
-      <c r="R15" s="41"/>
-    </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="H15" s="28"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="29"/>
+      <c r="M15" s="40"/>
+      <c r="R15" s="37"/>
+    </row>
+    <row r="16" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C16" s="24"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="35" t="s">
+      <c r="D16" s="28"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="31" t="s">
         <v>396</v>
       </c>
-      <c r="H16" s="32"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="33"/>
-      <c r="M16" s="45" t="s">
+      <c r="H16" s="28"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="29"/>
+      <c r="M16" s="41" t="s">
         <v>423</v>
       </c>
-      <c r="R16" s="40" t="s">
+      <c r="R16" s="36" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C17" s="24" t="s">
         <v>402</v>
       </c>
-      <c r="D17" s="32"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="35" t="s">
+      <c r="D17" s="28"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="31" t="s">
         <v>399</v>
       </c>
-      <c r="H17" s="32"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="34"/>
-      <c r="M17" s="44" t="s">
+      <c r="H17" s="28"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="30"/>
+      <c r="M17" s="40" t="s">
         <v>422</v>
       </c>
-      <c r="R17" s="42" t="s">
+      <c r="R17" s="38" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C18" s="24"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="35" t="s">
+      <c r="D18" s="28"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="31" t="s">
         <v>398</v>
       </c>
-      <c r="H18" s="32"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="34"/>
-      <c r="M18" s="47" t="s">
+      <c r="H18" s="28"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="30"/>
+      <c r="M18" s="43" t="s">
         <v>410</v>
       </c>
-      <c r="R18" s="50" t="s">
+      <c r="R18" s="46" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C19" s="24" t="s">
         <v>407</v>
       </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="34"/>
-      <c r="M19" s="47" t="s">
+      <c r="D19" s="28"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="30"/>
+      <c r="M19" s="43" t="s">
         <v>411</v>
       </c>
-      <c r="R19" s="50" t="s">
+      <c r="R19" s="46" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C20" s="36" t="s">
+    <row r="20" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C20" s="32" t="s">
         <v>408</v>
       </c>
-      <c r="D20" s="32"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32" t="s">
+      <c r="D20" s="28"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28" t="s">
         <v>404</v>
       </c>
-      <c r="H20" s="32"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="34"/>
-      <c r="M20" s="47" t="s">
+      <c r="H20" s="28"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="30"/>
+      <c r="M20" s="43" t="s">
         <v>412</v>
       </c>
-      <c r="R20" s="50" t="s">
+      <c r="R20" s="46" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C21" s="24"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="35" t="s">
+      <c r="D21" s="28"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="31" t="s">
         <v>397</v>
       </c>
-      <c r="H21" s="32"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="33"/>
-      <c r="M21" s="48" t="s">
+      <c r="H21" s="28"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="29"/>
+      <c r="M21" s="44" t="s">
         <v>413</v>
       </c>
-      <c r="R21" s="49" t="s">
+      <c r="R21" s="45" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C22" s="24"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="35" t="s">
+      <c r="D22" s="28"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="31" t="s">
         <v>406</v>
       </c>
-      <c r="H22" s="32"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="33"/>
-      <c r="M22" s="44"/>
-      <c r="R22" s="41"/>
-    </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="H22" s="28"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="29"/>
+      <c r="M22" s="40"/>
+      <c r="R22" s="37"/>
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C23" s="24"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="35" t="s">
+      <c r="D23" s="28"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="31" t="s">
         <v>406</v>
       </c>
-      <c r="H23" s="32"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="33" t="s">
+      <c r="H23" s="28"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="29" t="s">
         <v>423</v>
       </c>
-      <c r="M23" s="45" t="s">
+      <c r="M23" s="41" t="s">
         <v>423</v>
       </c>
-      <c r="R23" s="40" t="s">
+      <c r="R23" s="36" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C24" s="24"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="35" t="s">
+      <c r="D24" s="28"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="31" t="s">
         <v>406</v>
       </c>
-      <c r="H24" s="32"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="33" t="s">
+      <c r="H24" s="28"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="29" t="s">
         <v>414</v>
       </c>
-      <c r="M24" s="44" t="s">
+      <c r="M24" s="40" t="s">
         <v>414</v>
       </c>
-      <c r="R24" s="42" t="s">
+      <c r="R24" s="38" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C25" s="24"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="34" t="s">
+      <c r="D25" s="28"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="30" t="s">
         <v>410</v>
       </c>
-      <c r="M25" s="47" t="s">
+      <c r="M25" s="43" t="s">
         <v>410</v>
       </c>
-      <c r="R25" s="50" t="s">
+      <c r="R25" s="46" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C26" s="24"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32" t="s">
+      <c r="D26" s="28"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28" t="s">
         <v>405</v>
       </c>
-      <c r="H26" s="32"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="34" t="s">
+      <c r="H26" s="28"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="30" t="s">
         <v>411</v>
       </c>
-      <c r="M26" s="47" t="s">
+      <c r="M26" s="43" t="s">
         <v>411</v>
       </c>
-      <c r="R26" s="50" t="s">
+      <c r="R26" s="46" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="27" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C27" s="24"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="34" t="s">
+      <c r="D27" s="28"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="30" t="s">
         <v>412</v>
       </c>
-      <c r="M27" s="47" t="s">
+      <c r="M27" s="43" t="s">
         <v>412</v>
       </c>
-      <c r="R27" s="50" t="s">
+      <c r="R27" s="46" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C28" s="24"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="34" t="s">
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="30" t="s">
         <v>413</v>
       </c>
-      <c r="M28" s="48" t="s">
+      <c r="M28" s="44" t="s">
         <v>413</v>
       </c>
-      <c r="R28" s="49" t="s">
+      <c r="R28" s="45" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="29" spans="3:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C29" s="24"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="33"/>
-      <c r="M29" s="46"/>
-    </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="29"/>
+      <c r="M29" s="42"/>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C30" s="24"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="33" t="s">
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="29" t="s">
         <v>415</v>
       </c>
-      <c r="R30" s="41"/>
-    </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="R30" s="37"/>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C31" s="24"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="34" t="s">
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="30" t="s">
         <v>416</v>
       </c>
-      <c r="R31" s="41"/>
-    </row>
-    <row r="32" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="R31" s="37"/>
+    </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C32" s="24"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="34" t="s">
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="30" t="s">
         <v>417</v>
       </c>
-      <c r="R32" s="41"/>
-    </row>
-    <row r="33" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="R32" s="37"/>
+    </row>
+    <row r="33" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C33" s="24"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="34" t="s">
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="30" t="s">
         <v>418</v>
       </c>
-      <c r="R33" s="41"/>
-    </row>
-    <row r="34" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="R33" s="37"/>
+    </row>
+    <row r="34" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C34" s="24"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="34" t="s">
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="30" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="35" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C35" s="24"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="34" t="s">
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="30" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="36" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C36" s="37"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="38"/>
-      <c r="I36" s="38"/>
-      <c r="J36" s="38"/>
-      <c r="K36" s="39"/>
+    <row r="36" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C36" s="33"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4155,12 +4155,12 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>153</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>154</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>156</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>158</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>152</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>0</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -4399,23 +4399,23 @@
       <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" ht="58.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="25" t="s">
+    <row r="3" spans="1:8" ht="58.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="50" t="s">
         <v>159</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-    </row>
-    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.2">
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+    </row>
+    <row r="4" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>391</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>106</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>130</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>5</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>6</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>9</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>119</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>11</v>
       </c>
@@ -4717,7 +4717,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>12</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>131</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>13</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>14</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>113</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>15</v>
       </c>
@@ -4867,7 +4867,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>16</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>19</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>20</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>132</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>114</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>23</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>24</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -5173,7 +5173,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>128</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>107</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>37</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>38</v>
       </c>
@@ -5271,7 +5271,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>120</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -5320,7 +5320,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>129</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>108</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>44</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>45</v>
       </c>
@@ -5444,7 +5444,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>46</v>
       </c>
@@ -5470,7 +5470,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>47</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>48</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>49</v>
       </c>
@@ -5548,7 +5548,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>50</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>109</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -5623,7 +5623,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -5673,7 +5673,7 @@
       </c>
       <c r="H54" s="23"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>59</v>
       </c>
@@ -5697,7 +5697,7 @@
       </c>
       <c r="H55" s="23"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>60</v>
       </c>
@@ -5721,7 +5721,7 @@
       </c>
       <c r="H56" s="24"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>61</v>
       </c>
@@ -5744,7 +5744,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>62</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>110</v>
       </c>
@@ -5790,7 +5790,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>63</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>64</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>126</v>
       </c>
@@ -5859,7 +5859,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>65</v>
       </c>
@@ -5882,7 +5882,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>66</v>
       </c>
@@ -5905,7 +5905,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>121</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>67</v>
       </c>
@@ -5951,7 +5951,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>68</v>
       </c>
@@ -5974,7 +5974,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>70</v>
       </c>
@@ -5997,7 +5997,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>71</v>
       </c>
@@ -6020,7 +6020,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>72</v>
       </c>
@@ -6043,7 +6043,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>127</v>
       </c>
@@ -6066,7 +6066,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>74</v>
       </c>
@@ -6089,7 +6089,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>75</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>111</v>
       </c>
@@ -6135,7 +6135,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>76</v>
       </c>
@@ -6158,7 +6158,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>77</v>
       </c>
@@ -6181,7 +6181,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>78</v>
       </c>
@@ -6204,7 +6204,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>79</v>
       </c>
@@ -6227,7 +6227,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>80</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>81</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>122</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>82</v>
       </c>
@@ -6319,7 +6319,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>83</v>
       </c>
@@ -6342,7 +6342,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>84</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>86</v>
       </c>
@@ -6388,7 +6388,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>87</v>
       </c>
@@ -6411,7 +6411,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>88</v>
       </c>
@@ -6434,7 +6434,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>115</v>
       </c>
@@ -6457,7 +6457,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>89</v>
       </c>
@@ -6480,7 +6480,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>90</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>91</v>
       </c>
@@ -6526,7 +6526,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>125</v>
       </c>
@@ -6549,7 +6549,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>93</v>
       </c>
@@ -6572,7 +6572,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>94</v>
       </c>
@@ -6595,7 +6595,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>95</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>124</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -6664,7 +6664,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -6710,7 +6710,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -6733,7 +6733,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -6756,7 +6756,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>112</v>
       </c>
@@ -6779,7 +6779,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -6802,7 +6802,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" s="2">
         <v>104</v>
       </c>
@@ -6825,7 +6825,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="2">
         <v>7</v>
       </c>
@@ -6848,7 +6848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="2">
         <v>8</v>
       </c>
@@ -6871,7 +6871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="2">
         <v>17</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="2">
         <v>18</v>
       </c>
@@ -6917,7 +6917,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="2">
         <v>21</v>
       </c>
@@ -6940,7 +6940,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="2">
         <v>22</v>
       </c>
@@ -6963,7 +6963,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="2">
         <v>25</v>
       </c>
@@ -6986,7 +6986,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="2">
         <v>26</v>
       </c>
@@ -7009,7 +7009,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" s="2">
         <v>27</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="2">
         <v>28</v>
       </c>
@@ -7055,7 +7055,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="2">
         <v>34</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="2">
         <v>35</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="2">
         <v>36</v>
       </c>
@@ -7124,7 +7124,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="2">
         <v>41</v>
       </c>
@@ -7147,7 +7147,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" s="2">
         <v>42</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="2">
         <v>43</v>
       </c>
@@ -7193,7 +7193,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="2">
         <v>54</v>
       </c>
@@ -7216,7 +7216,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="2">
         <v>55</v>
       </c>
@@ -7239,7 +7239,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" s="2">
         <v>56</v>
       </c>
@@ -7262,7 +7262,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="2">
         <v>57</v>
       </c>
@@ -7285,7 +7285,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="2">
         <v>58</v>
       </c>
@@ -7308,7 +7308,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" s="2">
         <v>69</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="2">
         <v>73</v>
       </c>
@@ -7354,7 +7354,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" s="2">
         <v>85</v>
       </c>
@@ -7377,7 +7377,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" s="2">
         <v>92</v>
       </c>
@@ -7400,7 +7400,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" s="2">
         <v>101</v>
       </c>
@@ -7423,7 +7423,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="2">
         <v>103</v>
       </c>
@@ -7446,7 +7446,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" s="2">
         <v>105</v>
       </c>
@@ -7469,7 +7469,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" s="2">
         <v>116</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="2">
         <v>117</v>
       </c>
@@ -7515,7 +7515,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="2">
         <v>118</v>
       </c>
@@ -7538,7 +7538,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="2">
         <v>123</v>
       </c>
@@ -7561,7 +7561,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="2">
         <v>133</v>
       </c>
@@ -7584,7 +7584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" s="2">
         <v>134</v>
       </c>
@@ -7607,7 +7607,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="2">
         <v>135</v>
       </c>
@@ -7630,7 +7630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" s="2">
         <v>136</v>
       </c>
@@ -7653,7 +7653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="2">
         <v>137</v>
       </c>
@@ -7676,7 +7676,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" s="2">
         <v>138</v>
       </c>
@@ -7699,7 +7699,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" s="2">
         <v>139</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" s="2">
         <v>140</v>
       </c>
@@ -7745,7 +7745,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" s="2">
         <v>141</v>
       </c>
@@ -7768,7 +7768,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" s="2">
         <v>142</v>
       </c>
@@ -7791,7 +7791,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" s="2">
         <v>143</v>
       </c>
@@ -7814,7 +7814,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" s="2">
         <v>144</v>
       </c>
@@ -7837,7 +7837,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" s="2">
         <v>145</v>
       </c>
@@ -7860,7 +7860,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" s="2">
         <v>146</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" s="2">
         <v>147</v>
       </c>
@@ -7906,7 +7906,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" s="2">
         <v>148</v>
       </c>
@@ -7929,7 +7929,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" s="2">
         <v>149</v>
       </c>
@@ -7952,7 +7952,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" s="2">
         <v>150</v>
       </c>
@@ -7975,7 +7975,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" s="2">
         <v>151</v>
       </c>
@@ -8124,16 +8124,16 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="15"/>
-    <col min="2" max="2" width="71.1640625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="15"/>
+    <col min="1" max="1" width="8.81640625" style="15"/>
+    <col min="2" max="2" width="71.1796875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.36328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>86</v>
       </c>
@@ -8147,7 +8147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -8158,7 +8158,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -8172,7 +8172,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -8186,7 +8186,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -8200,7 +8200,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -8212,7 +8212,7 @@
       </c>
       <c r="D6" s="16"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -8220,7 +8220,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -8228,7 +8228,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -8242,7 +8242,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -8256,7 +8256,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -8267,7 +8267,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -8278,7 +8278,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -8289,7 +8289,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -8300,7 +8300,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -8308,7 +8308,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <v>15</v>
       </c>
@@ -8316,7 +8316,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -8327,7 +8327,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -8338,7 +8338,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -8349,7 +8349,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -8360,7 +8360,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -8371,7 +8371,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -8382,7 +8382,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -8393,7 +8393,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -8404,7 +8404,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -8415,7 +8415,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -8426,7 +8426,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -8437,7 +8437,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -8446,7 +8446,7 @@
       </c>
       <c r="D28" s="16"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -8457,7 +8457,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -8468,7 +8468,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -8476,7 +8476,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -8484,7 +8484,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -8495,7 +8495,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -8509,7 +8509,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -8523,7 +8523,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -8537,7 +8537,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -8551,7 +8551,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -8565,7 +8565,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -8579,7 +8579,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -8587,7 +8587,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -8595,7 +8595,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -8606,7 +8606,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -8620,7 +8620,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -8634,7 +8634,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -8645,12 +8645,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D47" s="18" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D48" s="16"/>
     </row>
   </sheetData>
@@ -8669,27 +8669,27 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" style="13" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" style="13"/>
-    <col min="4" max="4" width="10.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.6640625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="6.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.1640625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="6.1640625" style="13" customWidth="1"/>
-    <col min="10" max="11" width="8.83203125" style="13"/>
-    <col min="12" max="13" width="6.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="13"/>
+    <col min="1" max="1" width="27.1796875" style="13" customWidth="1"/>
+    <col min="2" max="3" width="8.81640625" style="13"/>
+    <col min="4" max="4" width="10.453125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6328125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="6.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.1796875" style="13" customWidth="1"/>
+    <col min="8" max="8" width="6.36328125" style="13" customWidth="1"/>
+    <col min="9" max="9" width="6.1796875" style="13" customWidth="1"/>
+    <col min="10" max="11" width="8.81640625" style="13"/>
+    <col min="12" max="13" width="6.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.81640625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E1" s="13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="119.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="119.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E2" s="17" t="s">
         <v>132</v>
       </c>
@@ -8718,7 +8718,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>80</v>
       </c>
@@ -8726,7 +8726,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
         <v>142</v>
       </c>
@@ -8749,7 +8749,7 @@
       <c r="L4" s="19"/>
       <c r="M4" s="19"/>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>83</v>
       </c>
@@ -8768,7 +8768,7 @@
       <c r="L5" s="19"/>
       <c r="M5" s="19"/>
     </row>
-    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>84</v>
       </c>
@@ -8787,7 +8787,7 @@
       <c r="L6" s="19"/>
       <c r="M6" s="19"/>
     </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>85</v>
       </c>
@@ -8806,7 +8806,7 @@
       <c r="L7" s="19"/>
       <c r="M7" s="19"/>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
         <v>143</v>
       </c>
@@ -8825,7 +8825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
         <v>145</v>
       </c>
@@ -8844,7 +8844,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
         <v>146</v>
       </c>
@@ -8865,7 +8865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>147</v>
       </c>
@@ -8886,7 +8886,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>144</v>
       </c>
@@ -8907,7 +8907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>148</v>
       </c>
@@ -8926,7 +8926,7 @@
       </c>
       <c r="M13" s="19"/>
     </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
         <v>149</v>
       </c>
@@ -8945,7 +8945,7 @@
       </c>
       <c r="M14" s="19"/>
     </row>
-    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>139</v>
       </c>
@@ -8966,7 +8966,7 @@
       </c>
       <c r="M15" s="19"/>
     </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>150</v>
       </c>
@@ -8983,7 +8983,7 @@
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>151</v>
       </c>
@@ -9000,7 +9000,7 @@
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E19" s="13">
         <f>SUMPRODUCT($D4:$D17, E4:E17)</f>
         <v>40</v>

</xml_diff>

<commit_message>
Add L2 requirements. Add FPGA concept drawing.
</commit_message>
<xml_diff>
--- a/01-requirements/Requirements Analysis.xlsx
+++ b/01-requirements/Requirements Analysis.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korwinula\Documents\MIDI-Router\01-requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\sandbox\MIDI-Router\01-requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0BFE3CB5-DF6E-4CAE-8275-201822F71AEA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30120" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="30120" windowHeight="21000" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="System Diagram" sheetId="6" r:id="rId1"/>
@@ -18,6 +17,8 @@
     <sheet name="FPGA Pin Use" sheetId="5" r:id="rId3"/>
     <sheet name="PIC24" sheetId="4" r:id="rId4"/>
     <sheet name="Requirements-QFD1" sheetId="3" r:id="rId5"/>
+    <sheet name="FPGA Requirements-QFD2" sheetId="7" r:id="rId6"/>
+    <sheet name="MCU Requirements-QFD2" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'FPGA Pin Use'!$A$4:$H$155</definedName>
@@ -32,12 +33,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Korwin</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{5C38E5A9-A3C5-4A1D-A317-C94D68D92895}">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{489C4BA3-E530-4BA9-B505-D2DB433771A1}">
+    <comment ref="A11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="428">
   <si>
     <t>Pin Count</t>
   </si>
@@ -1359,12 +1360,15 @@
   </si>
   <si>
     <t>120 VAC</t>
+  </si>
+  <si>
+    <t>Requirement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1718,7 +1722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1829,6 +1833,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3554,20 +3561,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8268F9F-964F-594F-B2B4-2D91C8B5EC04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="10.81640625" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C4" s="25"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -3578,7 +3585,7 @@
       <c r="J4" s="26"/>
       <c r="K4" s="27"/>
     </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C5" s="24"/>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
@@ -3592,7 +3599,7 @@
       </c>
       <c r="M5" s="28"/>
     </row>
-    <row r="6" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="24"/>
       <c r="D6" s="28"/>
       <c r="E6" s="28"/>
@@ -3609,7 +3616,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C7" s="24"/>
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
@@ -3628,7 +3635,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C8" s="24"/>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
@@ -3640,7 +3647,7 @@
       <c r="K8" s="29"/>
       <c r="M8" s="40"/>
     </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C9" s="24"/>
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
@@ -3659,7 +3666,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C10" s="24"/>
       <c r="D10" s="28"/>
       <c r="E10" s="28"/>
@@ -3680,7 +3687,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C11" s="24"/>
       <c r="D11" s="28"/>
       <c r="E11" s="47" t="s">
@@ -3703,7 +3710,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C12" s="24"/>
       <c r="D12" s="28"/>
       <c r="E12" s="48"/>
@@ -3724,7 +3731,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C13" s="24"/>
       <c r="D13" s="28"/>
       <c r="E13" s="48"/>
@@ -3745,7 +3752,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C14" s="24"/>
       <c r="D14" s="28"/>
       <c r="E14" s="48"/>
@@ -3764,7 +3771,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C15" s="24"/>
       <c r="D15" s="28"/>
       <c r="E15" s="48"/>
@@ -3779,7 +3786,7 @@
       <c r="M15" s="40"/>
       <c r="R15" s="37"/>
     </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C16" s="24"/>
       <c r="D16" s="28"/>
       <c r="E16" s="48"/>
@@ -3798,7 +3805,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C17" s="24" t="s">
         <v>402</v>
       </c>
@@ -3819,7 +3826,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C18" s="24"/>
       <c r="D18" s="28"/>
       <c r="E18" s="48"/>
@@ -3838,7 +3845,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C19" s="24" t="s">
         <v>407</v>
       </c>
@@ -3857,7 +3864,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C20" s="32" t="s">
         <v>408</v>
       </c>
@@ -3878,7 +3885,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C21" s="24"/>
       <c r="D21" s="28"/>
       <c r="E21" s="48"/>
@@ -3897,7 +3904,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C22" s="24"/>
       <c r="D22" s="28"/>
       <c r="E22" s="48"/>
@@ -3912,7 +3919,7 @@
       <c r="M22" s="40"/>
       <c r="R22" s="37"/>
     </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C23" s="24"/>
       <c r="D23" s="28"/>
       <c r="E23" s="48"/>
@@ -3933,7 +3940,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C24" s="24"/>
       <c r="D24" s="28"/>
       <c r="E24" s="48"/>
@@ -3954,7 +3961,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C25" s="24"/>
       <c r="D25" s="28"/>
       <c r="E25" s="48"/>
@@ -3973,7 +3980,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C26" s="24"/>
       <c r="D26" s="28"/>
       <c r="E26" s="48"/>
@@ -3994,7 +4001,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="27" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C27" s="24"/>
       <c r="D27" s="28"/>
       <c r="E27" s="49"/>
@@ -4013,7 +4020,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C28" s="24"/>
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
@@ -4032,7 +4039,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="29" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="24"/>
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
@@ -4044,7 +4051,7 @@
       <c r="K29" s="29"/>
       <c r="M29" s="42"/>
     </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C30" s="24"/>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
@@ -4058,7 +4065,7 @@
       </c>
       <c r="R30" s="37"/>
     </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C31" s="24"/>
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
@@ -4072,7 +4079,7 @@
       </c>
       <c r="R31" s="37"/>
     </row>
-    <row r="32" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C32" s="24"/>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
@@ -4086,7 +4093,7 @@
       </c>
       <c r="R32" s="37"/>
     </row>
-    <row r="33" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C33" s="24"/>
       <c r="D33" s="28"/>
       <c r="E33" s="28"/>
@@ -4100,7 +4107,7 @@
       </c>
       <c r="R33" s="37"/>
     </row>
-    <row r="34" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C34" s="24"/>
       <c r="D34" s="28"/>
       <c r="E34" s="28"/>
@@ -4113,7 +4120,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="35" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C35" s="24"/>
       <c r="D35" s="28"/>
       <c r="E35" s="28"/>
@@ -4126,7 +4133,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="36" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C36" s="33"/>
       <c r="D36" s="34"/>
       <c r="E36" s="34"/>
@@ -4148,19 +4155,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4174,7 +4181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4190,7 +4197,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>153</v>
       </c>
@@ -4205,7 +4212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>154</v>
       </c>
@@ -4220,7 +4227,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -4235,7 +4242,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>156</v>
       </c>
@@ -4250,7 +4257,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -4265,7 +4272,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>158</v>
       </c>
@@ -4280,7 +4287,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>152</v>
       </c>
@@ -4295,7 +4302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -4310,7 +4317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -4326,7 +4333,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0</v>
       </c>
@@ -4338,7 +4345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -4353,7 +4360,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -4362,7 +4369,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -4370,7 +4377,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -4387,7 +4394,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63F63D7-D9E5-44DC-B22E-D22BA96211A0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A3:H155"/>
   <sheetViews>
@@ -4399,13 +4406,13 @@
       <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" ht="58.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="58.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="50" t="s">
         <v>159</v>
       </c>
@@ -4415,7 +4422,7 @@
       <c r="F3" s="50"/>
       <c r="G3" s="50"/>
     </row>
-    <row r="4" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>391</v>
       </c>
@@ -4441,7 +4448,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -4464,7 +4471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -4487,7 +4494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -4510,7 +4517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -4533,7 +4540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>106</v>
       </c>
@@ -4556,7 +4563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>130</v>
       </c>
@@ -4579,7 +4586,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>5</v>
       </c>
@@ -4602,7 +4609,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>6</v>
       </c>
@@ -4625,7 +4632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>9</v>
       </c>
@@ -4648,7 +4655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -4671,7 +4678,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>119</v>
       </c>
@@ -4694,7 +4701,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>11</v>
       </c>
@@ -4717,7 +4724,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>12</v>
       </c>
@@ -4743,7 +4750,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>131</v>
       </c>
@@ -4766,7 +4773,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>13</v>
       </c>
@@ -4792,7 +4799,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>14</v>
       </c>
@@ -4818,7 +4825,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>113</v>
       </c>
@@ -4841,7 +4848,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>15</v>
       </c>
@@ -4867,7 +4874,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>16</v>
       </c>
@@ -4893,7 +4900,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>19</v>
       </c>
@@ -4919,7 +4926,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>20</v>
       </c>
@@ -4945,7 +4952,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>132</v>
       </c>
@@ -4968,7 +4975,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>114</v>
       </c>
@@ -4991,7 +4998,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>23</v>
       </c>
@@ -5017,7 +5024,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>24</v>
       </c>
@@ -5043,7 +5050,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -5069,7 +5076,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -5095,7 +5102,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -5121,7 +5128,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -5147,7 +5154,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -5173,7 +5180,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>128</v>
       </c>
@@ -5196,7 +5203,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>107</v>
       </c>
@@ -5219,7 +5226,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>37</v>
       </c>
@@ -5245,7 +5252,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>38</v>
       </c>
@@ -5271,7 +5278,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>120</v>
       </c>
@@ -5294,7 +5301,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -5320,7 +5327,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -5346,7 +5353,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>129</v>
       </c>
@@ -5369,7 +5376,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>108</v>
       </c>
@@ -5392,7 +5399,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>44</v>
       </c>
@@ -5418,7 +5425,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>45</v>
       </c>
@@ -5444,7 +5451,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>46</v>
       </c>
@@ -5470,7 +5477,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>47</v>
       </c>
@@ -5496,7 +5503,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>48</v>
       </c>
@@ -5522,7 +5529,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>49</v>
       </c>
@@ -5548,7 +5555,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>50</v>
       </c>
@@ -5574,7 +5581,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>109</v>
       </c>
@@ -5597,7 +5604,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -5623,7 +5630,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -5649,7 +5656,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -5673,7 +5680,7 @@
       </c>
       <c r="H54" s="23"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>59</v>
       </c>
@@ -5697,7 +5704,7 @@
       </c>
       <c r="H55" s="23"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>60</v>
       </c>
@@ -5721,7 +5728,7 @@
       </c>
       <c r="H56" s="24"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>61</v>
       </c>
@@ -5744,7 +5751,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>62</v>
       </c>
@@ -5767,7 +5774,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>110</v>
       </c>
@@ -5790,7 +5797,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>63</v>
       </c>
@@ -5813,7 +5820,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>64</v>
       </c>
@@ -5836,7 +5843,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>126</v>
       </c>
@@ -5859,7 +5866,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>65</v>
       </c>
@@ -5882,7 +5889,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>66</v>
       </c>
@@ -5905,7 +5912,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>121</v>
       </c>
@@ -5928,7 +5935,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>67</v>
       </c>
@@ -5951,7 +5958,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>68</v>
       </c>
@@ -5974,7 +5981,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>70</v>
       </c>
@@ -5997,7 +6004,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>71</v>
       </c>
@@ -6020,7 +6027,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>72</v>
       </c>
@@ -6043,7 +6050,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>127</v>
       </c>
@@ -6066,7 +6073,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>74</v>
       </c>
@@ -6089,7 +6096,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>75</v>
       </c>
@@ -6112,7 +6119,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>111</v>
       </c>
@@ -6135,7 +6142,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>76</v>
       </c>
@@ -6158,7 +6165,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>77</v>
       </c>
@@ -6181,7 +6188,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>78</v>
       </c>
@@ -6204,7 +6211,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>79</v>
       </c>
@@ -6227,7 +6234,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>80</v>
       </c>
@@ -6250,7 +6257,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>81</v>
       </c>
@@ -6273,7 +6280,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>122</v>
       </c>
@@ -6296,7 +6303,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>82</v>
       </c>
@@ -6319,7 +6326,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>83</v>
       </c>
@@ -6342,7 +6349,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>84</v>
       </c>
@@ -6365,7 +6372,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>86</v>
       </c>
@@ -6388,7 +6395,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>87</v>
       </c>
@@ -6411,7 +6418,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>88</v>
       </c>
@@ -6434,7 +6441,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>115</v>
       </c>
@@ -6457,7 +6464,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>89</v>
       </c>
@@ -6480,7 +6487,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>90</v>
       </c>
@@ -6503,7 +6510,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>91</v>
       </c>
@@ -6526,7 +6533,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>125</v>
       </c>
@@ -6549,7 +6556,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>93</v>
       </c>
@@ -6572,7 +6579,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>94</v>
       </c>
@@ -6595,7 +6602,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>95</v>
       </c>
@@ -6618,7 +6625,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>124</v>
       </c>
@@ -6641,7 +6648,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -6664,7 +6671,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -6687,7 +6694,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -6710,7 +6717,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -6733,7 +6740,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -6756,7 +6763,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>112</v>
       </c>
@@ -6779,7 +6786,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -6802,7 +6809,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>104</v>
       </c>
@@ -6825,7 +6832,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>7</v>
       </c>
@@ -6848,7 +6855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>8</v>
       </c>
@@ -6871,7 +6878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>17</v>
       </c>
@@ -6894,7 +6901,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>18</v>
       </c>
@@ -6917,7 +6924,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>21</v>
       </c>
@@ -6940,7 +6947,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>22</v>
       </c>
@@ -6963,7 +6970,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>25</v>
       </c>
@@ -6986,7 +6993,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>26</v>
       </c>
@@ -7009,7 +7016,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>27</v>
       </c>
@@ -7032,7 +7039,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>28</v>
       </c>
@@ -7055,7 +7062,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>34</v>
       </c>
@@ -7078,7 +7085,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>35</v>
       </c>
@@ -7101,7 +7108,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>36</v>
       </c>
@@ -7124,7 +7131,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>41</v>
       </c>
@@ -7147,7 +7154,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>42</v>
       </c>
@@ -7170,7 +7177,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>43</v>
       </c>
@@ -7193,7 +7200,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>54</v>
       </c>
@@ -7216,7 +7223,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>55</v>
       </c>
@@ -7239,7 +7246,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>56</v>
       </c>
@@ -7262,7 +7269,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>57</v>
       </c>
@@ -7285,7 +7292,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>58</v>
       </c>
@@ -7308,7 +7315,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>69</v>
       </c>
@@ -7331,7 +7338,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>73</v>
       </c>
@@ -7354,7 +7361,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>85</v>
       </c>
@@ -7377,7 +7384,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>92</v>
       </c>
@@ -7400,7 +7407,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>101</v>
       </c>
@@ -7423,7 +7430,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>103</v>
       </c>
@@ -7446,7 +7453,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>105</v>
       </c>
@@ -7469,7 +7476,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>116</v>
       </c>
@@ -7492,7 +7499,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>117</v>
       </c>
@@ -7515,7 +7522,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>118</v>
       </c>
@@ -7538,7 +7545,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>123</v>
       </c>
@@ -7561,7 +7568,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>133</v>
       </c>
@@ -7584,7 +7591,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>134</v>
       </c>
@@ -7607,7 +7614,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>135</v>
       </c>
@@ -7630,7 +7637,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>136</v>
       </c>
@@ -7653,7 +7660,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>137</v>
       </c>
@@ -7676,7 +7683,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>138</v>
       </c>
@@ -7699,7 +7706,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>139</v>
       </c>
@@ -7722,7 +7729,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>140</v>
       </c>
@@ -7745,7 +7752,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>141</v>
       </c>
@@ -7768,7 +7775,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>142</v>
       </c>
@@ -7791,7 +7798,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>143</v>
       </c>
@@ -7814,7 +7821,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>144</v>
       </c>
@@ -7837,7 +7844,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>145</v>
       </c>
@@ -7860,7 +7867,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>146</v>
       </c>
@@ -7883,7 +7890,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>147</v>
       </c>
@@ -7906,7 +7913,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>148</v>
       </c>
@@ -7929,7 +7936,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>149</v>
       </c>
@@ -7952,7 +7959,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>150</v>
       </c>
@@ -7975,7 +7982,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>151</v>
       </c>
@@ -7999,7 +8006,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:H155" xr:uid="{509DC822-51B5-42C9-8881-B0941EE9B587}">
+  <autoFilter ref="A4:H155">
     <filterColumn colId="4">
       <filters>
         <filter val="1"/>
@@ -8117,23 +8124,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="15"/>
-    <col min="2" max="2" width="71.1796875" style="15" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.36328125" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="15"/>
+    <col min="1" max="1" width="8.85546875" style="15"/>
+    <col min="2" max="2" width="71.140625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>86</v>
       </c>
@@ -8147,7 +8154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -8158,7 +8165,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -8172,7 +8179,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -8186,7 +8193,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -8200,7 +8207,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -8212,7 +8219,7 @@
       </c>
       <c r="D6" s="16"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -8220,7 +8227,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -8228,7 +8235,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -8242,7 +8249,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -8256,7 +8263,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -8267,7 +8274,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -8278,7 +8285,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -8289,7 +8296,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -8300,7 +8307,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -8308,7 +8315,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>15</v>
       </c>
@@ -8316,7 +8323,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -8327,7 +8334,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -8338,7 +8345,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -8349,7 +8356,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -8360,7 +8367,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -8371,7 +8378,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -8382,7 +8389,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -8393,7 +8400,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -8404,7 +8411,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -8415,7 +8422,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -8426,7 +8433,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -8437,7 +8444,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -8446,7 +8453,7 @@
       </c>
       <c r="D28" s="16"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -8457,7 +8464,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -8468,7 +8475,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -8476,7 +8483,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -8484,7 +8491,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -8495,7 +8502,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -8509,7 +8516,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -8523,7 +8530,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -8537,7 +8544,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -8551,7 +8558,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -8565,7 +8572,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -8579,7 +8586,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -8587,7 +8594,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -8595,7 +8602,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -8606,7 +8613,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -8620,7 +8627,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -8634,7 +8641,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -8645,12 +8652,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="D47" s="18" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D48" s="16"/>
     </row>
   </sheetData>
@@ -8659,37 +8666,37 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" style="13" customWidth="1"/>
-    <col min="2" max="3" width="8.81640625" style="13"/>
-    <col min="4" max="4" width="10.453125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.6328125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="6.1796875" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.1796875" style="13" customWidth="1"/>
-    <col min="8" max="8" width="6.36328125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="6.1796875" style="13" customWidth="1"/>
-    <col min="10" max="11" width="8.81640625" style="13"/>
-    <col min="12" max="13" width="6.1796875" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.81640625" style="13"/>
+    <col min="1" max="1" width="27.140625" style="13" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="13"/>
+    <col min="4" max="4" width="10.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.140625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" style="13" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" style="13" customWidth="1"/>
+    <col min="10" max="11" width="8.85546875" style="13"/>
+    <col min="12" max="13" width="6.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E1" s="13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="119.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="119.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="17" t="s">
         <v>132</v>
       </c>
@@ -8718,7 +8725,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>80</v>
       </c>
@@ -8726,7 +8733,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>142</v>
       </c>
@@ -8749,7 +8756,7 @@
       <c r="L4" s="19"/>
       <c r="M4" s="19"/>
     </row>
-    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>83</v>
       </c>
@@ -8768,7 +8775,7 @@
       <c r="L5" s="19"/>
       <c r="M5" s="19"/>
     </row>
-    <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>84</v>
       </c>
@@ -8787,7 +8794,7 @@
       <c r="L6" s="19"/>
       <c r="M6" s="19"/>
     </row>
-    <row r="7" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>85</v>
       </c>
@@ -8806,7 +8813,7 @@
       <c r="L7" s="19"/>
       <c r="M7" s="19"/>
     </row>
-    <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>143</v>
       </c>
@@ -8825,7 +8832,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>145</v>
       </c>
@@ -8844,7 +8851,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>146</v>
       </c>
@@ -8865,7 +8872,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>147</v>
       </c>
@@ -8886,7 +8893,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>144</v>
       </c>
@@ -8907,7 +8914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>148</v>
       </c>
@@ -8926,7 +8933,7 @@
       </c>
       <c r="M13" s="19"/>
     </row>
-    <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>149</v>
       </c>
@@ -8945,7 +8952,7 @@
       </c>
       <c r="M14" s="19"/>
     </row>
-    <row r="15" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>139</v>
       </c>
@@ -8966,7 +8973,7 @@
       </c>
       <c r="M15" s="19"/>
     </row>
-    <row r="16" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>150</v>
       </c>
@@ -8983,7 +8990,7 @@
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>151</v>
       </c>
@@ -9000,7 +9007,7 @@
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E19" s="13">
         <f>SUMPRODUCT($D4:$D17, E4:E17)</f>
         <v>40</v>
@@ -9042,4 +9049,116 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="51" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="51" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="51" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="51" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="51" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="51" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="51" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="51" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="51" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="51"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="51"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="51"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="51"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="51"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="51"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>